<commit_message>
Update course including course project
</commit_message>
<xml_diff>
--- a/docs/_static/FormatoPlaneacionInteractivos22023-10.xlsx
+++ b/docs/_static/FormatoPlaneacionInteractivos22023-10.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250456CA-CDC8-4DE5-86FC-0AAC3177C3D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47910AE-E749-4CB1-BA70-29A3334D6D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="72">
   <si>
     <t>PROYECTO DOCENTE</t>
   </si>
@@ -326,12 +326,6 @@
     <t>Versión del curso del semestre anterior. No se verifica, se deja solo como referencia para consulta en caso de ser necesario</t>
   </si>
   <si>
-    <t>1 h 40 min. Presentación del curso</t>
-  </si>
-  <si>
-    <t>Formativa</t>
-  </si>
-  <si>
     <t>Sumativa</t>
   </si>
   <si>
@@ -350,40 +344,34 @@
     <t>https://sistemasfisicosinteractivos2.readthedocs.io/</t>
   </si>
   <si>
-    <t>Unidad 1: comunicaciones seriales</t>
-  </si>
-  <si>
-    <t>1 h 40 min. Revisión de avances en la unidad y solución de dudas</t>
-  </si>
-  <si>
-    <t>1 h 40 min. Sustentación de la Unidad</t>
-  </si>
-  <si>
-    <t>Unidad 2: sensores y actuadores inteligentes</t>
-  </si>
-  <si>
-    <t>Introducción al curso y evaluación sumativa sobre control de versión con Unity</t>
-  </si>
-  <si>
-    <t>4 h. Evaluación sobre control de versión con Unity</t>
-  </si>
-  <si>
-    <t>4 h. Solución de la evaluación</t>
-  </si>
-  <si>
-    <t>Unidad 3: sensores y actuadores inalámbricos</t>
-  </si>
-  <si>
-    <t>Unidad 4: aplicaciones interactivas distribuidas</t>
-  </si>
-  <si>
-    <t>4 h. Montaje en el portafolio de la entraga</t>
-  </si>
-  <si>
-    <t>4 h. Realización de los ejercicios de la unidad</t>
-  </si>
-  <si>
-    <t>4 h. Terminar ejercicios de la unidad y comenzar la solución de la evaluación de la unidad</t>
+    <t>Introducción al curso</t>
+  </si>
+  <si>
+    <t>1 h 40 min. Presentación del proyecto de curso</t>
+  </si>
+  <si>
+    <t>Prototipo 1</t>
+  </si>
+  <si>
+    <t>Prototipo 2</t>
+  </si>
+  <si>
+    <t>Prototipo 3</t>
+  </si>
+  <si>
+    <t>Prototipo 4</t>
+  </si>
+  <si>
+    <t>4 h. Construcción del prototipo</t>
+  </si>
+  <si>
+    <t>4 h. Documentación con pruebas de usuario</t>
+  </si>
+  <si>
+    <t>Asesoría/Avances</t>
+  </si>
+  <si>
+    <t>Portafolio</t>
   </si>
 </sst>
 </file>
@@ -1383,9 +1371,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1586,6 +1571,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2007,8 +1995,8 @@
   </sheetPr>
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C21" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" zoomScalePageLayoutView="30" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26:L29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="80" zoomScalePageLayoutView="30" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2016,14 +2004,14 @@
     <col min="1" max="1" width="37.453125" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.1796875" style="1" customWidth="1"/>
     <col min="3" max="3" width="30" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.26953125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6328125" style="1" customWidth="1"/>
     <col min="5" max="5" width="17.81640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.26953125" style="1" customWidth="1"/>
     <col min="7" max="7" width="21.36328125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.26953125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="11.453125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="30.26953125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="46.1796875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13" style="1" customWidth="1"/>
+    <col min="10" max="10" width="45.7265625" style="121" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="49.6328125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="25.81640625" style="1" customWidth="1"/>
     <col min="13" max="13" width="23" style="1" customWidth="1"/>
     <col min="14" max="14" width="20.26953125" style="1" customWidth="1"/>
@@ -2031,159 +2019,159 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="29.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="57"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="56"/>
     </row>
     <row r="2" spans="1:13" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="58" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59"/>
-      <c r="M2" s="60"/>
+      <c r="A2" s="57" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="59"/>
     </row>
     <row r="3" spans="1:13" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="62"/>
-      <c r="L3" s="62"/>
-      <c r="M3" s="63"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="62"/>
     </row>
     <row r="4" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="66"/>
-      <c r="L4" s="66"/>
-      <c r="M4" s="67"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="65"/>
+      <c r="M4" s="66"/>
     </row>
     <row r="5" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="68"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="69"/>
-      <c r="K5" s="70"/>
-      <c r="L5" s="70"/>
-      <c r="M5" s="71"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="68"/>
+      <c r="K5" s="69"/>
+      <c r="L5" s="69"/>
+      <c r="M5" s="70"/>
     </row>
     <row r="6" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="72" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" s="72"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="73"/>
-      <c r="H6" s="73"/>
-      <c r="I6" s="73"/>
-      <c r="J6" s="73"/>
-      <c r="K6" s="74"/>
-      <c r="L6" s="74"/>
-      <c r="M6" s="75"/>
+      <c r="B6" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="71"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="73"/>
+      <c r="L6" s="73"/>
+      <c r="M6" s="74"/>
     </row>
     <row r="7" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="76">
+      <c r="B7" s="75">
         <v>15917</v>
       </c>
-      <c r="C7" s="76"/>
-      <c r="D7" s="77"/>
-      <c r="E7" s="77"/>
-      <c r="F7" s="77"/>
-      <c r="G7" s="77"/>
-      <c r="H7" s="77"/>
-      <c r="I7" s="77"/>
-      <c r="J7" s="77"/>
-      <c r="K7" s="78"/>
-      <c r="L7" s="78"/>
-      <c r="M7" s="79"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="76"/>
+      <c r="I7" s="76"/>
+      <c r="J7" s="76"/>
+      <c r="K7" s="77"/>
+      <c r="L7" s="77"/>
+      <c r="M7" s="78"/>
     </row>
     <row r="8" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="87">
+      <c r="B8" s="86">
         <v>2</v>
       </c>
-      <c r="C8" s="88"/>
+      <c r="C8" s="87"/>
       <c r="D8" s="27" t="s">
         <v>33</v>
       </c>
       <c r="E8" s="9">
         <v>96</v>
       </c>
-      <c r="F8" s="92" t="s">
+      <c r="F8" s="91" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="92"/>
+      <c r="G8" s="91"/>
       <c r="H8" s="9">
         <v>64</v>
       </c>
-      <c r="I8" s="89" t="s">
+      <c r="I8" s="88" t="s">
         <v>31</v>
       </c>
-      <c r="J8" s="90"/>
-      <c r="K8" s="90"/>
-      <c r="L8" s="91"/>
+      <c r="J8" s="89"/>
+      <c r="K8" s="89"/>
+      <c r="L8" s="90"/>
       <c r="M8" s="10">
         <v>32</v>
       </c>
@@ -2192,20 +2180,20 @@
       <c r="A9" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="80" t="s">
+      <c r="B9" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="80"/>
-      <c r="D9" s="81"/>
-      <c r="E9" s="81"/>
-      <c r="F9" s="81"/>
-      <c r="G9" s="81"/>
-      <c r="H9" s="81"/>
-      <c r="I9" s="81"/>
-      <c r="J9" s="81"/>
-      <c r="K9" s="82"/>
-      <c r="L9" s="82"/>
-      <c r="M9" s="83"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="80"/>
+      <c r="E9" s="80"/>
+      <c r="F9" s="80"/>
+      <c r="G9" s="80"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="80"/>
+      <c r="J9" s="80"/>
+      <c r="K9" s="81"/>
+      <c r="L9" s="81"/>
+      <c r="M9" s="82"/>
     </row>
     <row r="10" spans="1:13" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="32" t="s">
@@ -2215,16 +2203,16 @@
         <v>43</v>
       </c>
       <c r="C10" s="28"/>
-      <c r="D10" s="84"/>
-      <c r="E10" s="84"/>
-      <c r="F10" s="84"/>
-      <c r="G10" s="84"/>
-      <c r="H10" s="84"/>
-      <c r="I10" s="84"/>
-      <c r="J10" s="84"/>
-      <c r="K10" s="85"/>
-      <c r="L10" s="85"/>
-      <c r="M10" s="86"/>
+      <c r="D10" s="83"/>
+      <c r="E10" s="83"/>
+      <c r="F10" s="83"/>
+      <c r="G10" s="83"/>
+      <c r="H10" s="83"/>
+      <c r="I10" s="83"/>
+      <c r="J10" s="83"/>
+      <c r="K10" s="84"/>
+      <c r="L10" s="84"/>
+      <c r="M10" s="85"/>
     </row>
     <row r="11" spans="1:13" s="6" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="52" t="s">
@@ -2233,7 +2221,7 @@
       <c r="B11" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="120" t="s">
+      <c r="C11" s="119" t="s">
         <v>44</v>
       </c>
       <c r="D11" s="50" t="s">
@@ -2260,7 +2248,7 @@
     <row r="12" spans="1:13" s="6" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="53"/>
       <c r="B12" s="45"/>
-      <c r="C12" s="121"/>
+      <c r="C12" s="120"/>
       <c r="D12" s="26" t="s">
         <v>5</v>
       </c>
@@ -2284,16 +2272,16 @@
       <c r="L12" s="47"/>
       <c r="M12" s="47"/>
     </row>
-    <row r="13" spans="1:13" ht="43" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="53"/>
       <c r="B13" s="14" t="s">
         <v>41</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
@@ -2301,429 +2289,379 @@
       <c r="H13" s="17"/>
       <c r="I13" s="18"/>
       <c r="J13" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K13" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="L13" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="M13" s="42">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="L13" s="20"/>
+      <c r="M13" s="42"/>
+    </row>
+    <row r="14" spans="1:13" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A14" s="53"/>
       <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="54" t="s">
-        <v>64</v>
-      </c>
+      <c r="C14" s="4"/>
       <c r="D14" s="7"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H14" s="8"/>
       <c r="I14" s="19"/>
       <c r="J14" s="21" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="K14" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="L14" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="M14" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="L14" s="20"/>
+      <c r="M14" s="42"/>
+    </row>
+    <row r="15" spans="1:13" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A15" s="53"/>
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="54"/>
+      <c r="C15" s="4"/>
       <c r="D15" s="7"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="4" t="s">
-        <v>65</v>
-      </c>
+      <c r="G15" s="4"/>
       <c r="H15" s="8"/>
-      <c r="I15" s="19"/>
+      <c r="I15" s="19" t="s">
+        <v>64</v>
+      </c>
       <c r="J15" s="21" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="K15" s="41" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L15" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M15" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A16" s="53"/>
       <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="54"/>
+      <c r="C16" s="4"/>
       <c r="D16" s="7"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H16" s="8"/>
       <c r="I16" s="19"/>
       <c r="J16" s="21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K16" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="L16" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="M16" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="25" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="L16" s="20"/>
+      <c r="M16" s="42"/>
+    </row>
+    <row r="17" spans="1:13" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A17" s="53"/>
       <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="54"/>
+      <c r="C17" s="4"/>
       <c r="D17" s="7"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="H17" s="8"/>
       <c r="I17" s="19"/>
       <c r="J17" s="21" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="K17" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="L17" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="M17" s="43">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="L17" s="20"/>
+      <c r="M17" s="43"/>
+    </row>
+    <row r="18" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="53"/>
       <c r="B18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="54" t="s">
-        <v>67</v>
-      </c>
+      <c r="C18" s="4"/>
       <c r="D18" s="7"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="4"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="H18" s="8"/>
-      <c r="I18" s="19"/>
       <c r="J18" s="21" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="K18" s="41" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L18" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M18" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A19" s="53"/>
       <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="54"/>
+      <c r="C19" s="4"/>
       <c r="D19" s="7"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H19" s="8"/>
       <c r="I19" s="19"/>
       <c r="J19" s="21" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="K19" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="L19" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="M19" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="L19" s="20"/>
+      <c r="M19" s="42"/>
+    </row>
+    <row r="20" spans="1:13" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A20" s="53"/>
       <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="54"/>
+      <c r="C20" s="4"/>
       <c r="D20" s="7"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H20" s="8"/>
       <c r="I20" s="19"/>
       <c r="J20" s="21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K20" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="L20" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="M20" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="25" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="L20" s="20"/>
+      <c r="M20" s="42"/>
+    </row>
+    <row r="21" spans="1:13" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A21" s="53"/>
       <c r="B21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="54"/>
+      <c r="C21" s="4"/>
       <c r="D21" s="7"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
-      <c r="G21" s="4" t="s">
+      <c r="G21" s="4"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="H21" s="8"/>
-      <c r="I21" s="19"/>
       <c r="J21" s="21" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="K21" s="41" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L21" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="M21" s="43">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="M21" s="42">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A22" s="53"/>
       <c r="B22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="54" t="s">
-        <v>71</v>
-      </c>
+      <c r="C22" s="4"/>
       <c r="D22" s="7"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H22" s="8"/>
       <c r="I22" s="19"/>
       <c r="J22" s="21" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="K22" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="L22" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="M22" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="L22" s="20"/>
+      <c r="M22" s="42"/>
+    </row>
+    <row r="23" spans="1:13" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A23" s="53"/>
       <c r="B23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="54"/>
+      <c r="C23" s="4"/>
       <c r="D23" s="7"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H23" s="8"/>
       <c r="I23" s="19"/>
       <c r="J23" s="21" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="K23" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="L23" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="M23" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="L23" s="20"/>
+      <c r="M23" s="42"/>
+    </row>
+    <row r="24" spans="1:13" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A24" s="53"/>
       <c r="B24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="54"/>
+      <c r="C24" s="4"/>
       <c r="D24" s="7"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H24" s="8"/>
-      <c r="I24" s="19"/>
+      <c r="I24" s="19" t="s">
+        <v>67</v>
+      </c>
       <c r="J24" s="21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K24" s="41" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L24" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M24" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="25" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A25" s="53"/>
       <c r="B25" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="54"/>
+      <c r="C25" s="4"/>
       <c r="D25" s="7"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="H25" s="8"/>
       <c r="I25" s="19"/>
       <c r="J25" s="21" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K25" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="L25" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="M25" s="43">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="L25" s="20"/>
+      <c r="M25" s="42"/>
+    </row>
+    <row r="26" spans="1:13" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A26" s="53"/>
       <c r="B26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="54" t="s">
-        <v>72</v>
-      </c>
+      <c r="C26" s="4"/>
       <c r="D26" s="7"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H26" s="8"/>
       <c r="I26" s="19"/>
       <c r="J26" s="21" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="K26" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="L26" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="M26" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="L26" s="20"/>
+      <c r="M26" s="42"/>
+    </row>
+    <row r="27" spans="1:13" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A27" s="53"/>
       <c r="B27" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="54"/>
+      <c r="C27" s="4"/>
       <c r="D27" s="7"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H27" s="8"/>
       <c r="I27" s="19"/>
       <c r="J27" s="21" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="K27" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="L27" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="M27" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="L27" s="20"/>
+      <c r="M27" s="42"/>
+    </row>
+    <row r="28" spans="1:13" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A28" s="53"/>
       <c r="B28" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="54"/>
+      <c r="C28" s="4"/>
       <c r="D28" s="7"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
-      <c r="G28" s="4" t="s">
-        <v>65</v>
-      </c>
+      <c r="G28" s="4"/>
       <c r="H28" s="8"/>
-      <c r="I28" s="19"/>
+      <c r="I28" s="19" t="s">
+        <v>71</v>
+      </c>
       <c r="J28" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K28" s="41" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L28" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M28" s="42">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2731,27 +2669,17 @@
       <c r="B29" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="54"/>
+      <c r="C29" s="4"/>
       <c r="D29" s="7"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
-      <c r="G29" s="4" t="s">
-        <v>66</v>
-      </c>
+      <c r="G29" s="4"/>
       <c r="H29" s="8"/>
       <c r="I29" s="19"/>
-      <c r="J29" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="K29" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="L29" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="M29" s="43">
-        <v>0.25</v>
-      </c>
+      <c r="J29" s="3"/>
+      <c r="K29" s="20"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="43"/>
     </row>
     <row r="30" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="53"/>
@@ -2791,163 +2719,163 @@
       <c r="A32" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="103" t="s">
+      <c r="B32" s="102" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="104"/>
-      <c r="D32" s="104"/>
-      <c r="E32" s="104"/>
-      <c r="F32" s="104"/>
-      <c r="G32" s="104"/>
-      <c r="H32" s="105"/>
+      <c r="C32" s="103"/>
+      <c r="D32" s="103"/>
+      <c r="E32" s="103"/>
+      <c r="F32" s="103"/>
+      <c r="G32" s="103"/>
+      <c r="H32" s="104"/>
       <c r="I32" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="J32" s="99" t="s">
+      <c r="J32" s="98" t="s">
         <v>36</v>
       </c>
-      <c r="K32" s="100"/>
-      <c r="L32" s="100"/>
-      <c r="M32" s="101"/>
+      <c r="K32" s="99"/>
+      <c r="L32" s="99"/>
+      <c r="M32" s="100"/>
     </row>
     <row r="33" spans="1:13" ht="55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="102"/>
-      <c r="B33" s="106" t="s">
-        <v>61</v>
-      </c>
-      <c r="C33" s="107"/>
-      <c r="D33" s="107"/>
-      <c r="E33" s="107"/>
-      <c r="F33" s="107"/>
-      <c r="G33" s="107"/>
-      <c r="H33" s="108"/>
+      <c r="A33" s="101"/>
+      <c r="B33" s="105" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="106"/>
+      <c r="D33" s="106"/>
+      <c r="E33" s="106"/>
+      <c r="F33" s="106"/>
+      <c r="G33" s="106"/>
+      <c r="H33" s="107"/>
       <c r="I33" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="J33" s="114" t="s">
+      <c r="J33" s="113" t="s">
         <v>54</v>
       </c>
-      <c r="K33" s="115"/>
-      <c r="L33" s="115"/>
-      <c r="M33" s="116"/>
+      <c r="K33" s="114"/>
+      <c r="L33" s="114"/>
+      <c r="M33" s="115"/>
     </row>
     <row r="34" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="102"/>
-      <c r="B34" s="109" t="s">
-        <v>62</v>
-      </c>
-      <c r="C34" s="110"/>
-      <c r="D34" s="110"/>
-      <c r="E34" s="110"/>
-      <c r="F34" s="110"/>
-      <c r="G34" s="110"/>
-      <c r="H34" s="111"/>
+      <c r="A34" s="101"/>
+      <c r="B34" s="108" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="109"/>
+      <c r="D34" s="109"/>
+      <c r="E34" s="109"/>
+      <c r="F34" s="109"/>
+      <c r="G34" s="109"/>
+      <c r="H34" s="110"/>
       <c r="I34" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="J34" s="117" t="s">
+      <c r="J34" s="116" t="s">
         <v>55</v>
       </c>
-      <c r="K34" s="118"/>
-      <c r="L34" s="118"/>
-      <c r="M34" s="119"/>
+      <c r="K34" s="117"/>
+      <c r="L34" s="117"/>
+      <c r="M34" s="118"/>
     </row>
     <row r="35" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="102"/>
-      <c r="B35" s="87"/>
-      <c r="C35" s="94"/>
-      <c r="D35" s="94"/>
-      <c r="E35" s="94"/>
-      <c r="F35" s="94"/>
-      <c r="G35" s="94"/>
-      <c r="H35" s="88"/>
+      <c r="A35" s="101"/>
+      <c r="B35" s="86"/>
+      <c r="C35" s="93"/>
+      <c r="D35" s="93"/>
+      <c r="E35" s="93"/>
+      <c r="F35" s="93"/>
+      <c r="G35" s="93"/>
+      <c r="H35" s="87"/>
       <c r="I35" s="33"/>
-      <c r="J35" s="93"/>
-      <c r="K35" s="94"/>
-      <c r="L35" s="94"/>
-      <c r="M35" s="95"/>
+      <c r="J35" s="92"/>
+      <c r="K35" s="93"/>
+      <c r="L35" s="93"/>
+      <c r="M35" s="94"/>
     </row>
     <row r="36" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="102"/>
-      <c r="B36" s="87"/>
-      <c r="C36" s="94"/>
-      <c r="D36" s="94"/>
-      <c r="E36" s="94"/>
-      <c r="F36" s="94"/>
-      <c r="G36" s="94"/>
-      <c r="H36" s="88"/>
+      <c r="A36" s="101"/>
+      <c r="B36" s="86"/>
+      <c r="C36" s="93"/>
+      <c r="D36" s="93"/>
+      <c r="E36" s="93"/>
+      <c r="F36" s="93"/>
+      <c r="G36" s="93"/>
+      <c r="H36" s="87"/>
       <c r="I36" s="33"/>
-      <c r="J36" s="93"/>
-      <c r="K36" s="94"/>
-      <c r="L36" s="94"/>
-      <c r="M36" s="95"/>
+      <c r="J36" s="92"/>
+      <c r="K36" s="93"/>
+      <c r="L36" s="93"/>
+      <c r="M36" s="94"/>
     </row>
     <row r="37" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="102"/>
-      <c r="B37" s="87"/>
-      <c r="C37" s="94"/>
-      <c r="D37" s="94"/>
-      <c r="E37" s="94"/>
-      <c r="F37" s="94"/>
-      <c r="G37" s="94"/>
-      <c r="H37" s="88"/>
+      <c r="A37" s="101"/>
+      <c r="B37" s="86"/>
+      <c r="C37" s="93"/>
+      <c r="D37" s="93"/>
+      <c r="E37" s="93"/>
+      <c r="F37" s="93"/>
+      <c r="G37" s="93"/>
+      <c r="H37" s="87"/>
       <c r="I37" s="33"/>
-      <c r="J37" s="93"/>
-      <c r="K37" s="94"/>
-      <c r="L37" s="94"/>
-      <c r="M37" s="95"/>
+      <c r="J37" s="92"/>
+      <c r="K37" s="93"/>
+      <c r="L37" s="93"/>
+      <c r="M37" s="94"/>
     </row>
     <row r="38" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="102"/>
-      <c r="B38" s="87"/>
-      <c r="C38" s="94"/>
-      <c r="D38" s="94"/>
-      <c r="E38" s="94"/>
-      <c r="F38" s="94"/>
-      <c r="G38" s="94"/>
-      <c r="H38" s="88"/>
+      <c r="A38" s="101"/>
+      <c r="B38" s="86"/>
+      <c r="C38" s="93"/>
+      <c r="D38" s="93"/>
+      <c r="E38" s="93"/>
+      <c r="F38" s="93"/>
+      <c r="G38" s="93"/>
+      <c r="H38" s="87"/>
       <c r="I38" s="33"/>
-      <c r="J38" s="93"/>
-      <c r="K38" s="94"/>
-      <c r="L38" s="94"/>
-      <c r="M38" s="95"/>
+      <c r="J38" s="92"/>
+      <c r="K38" s="93"/>
+      <c r="L38" s="93"/>
+      <c r="M38" s="94"/>
     </row>
     <row r="39" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="102"/>
-      <c r="B39" s="87"/>
-      <c r="C39" s="94"/>
-      <c r="D39" s="94"/>
-      <c r="E39" s="94"/>
-      <c r="F39" s="94"/>
-      <c r="G39" s="94"/>
-      <c r="H39" s="88"/>
+      <c r="A39" s="101"/>
+      <c r="B39" s="86"/>
+      <c r="C39" s="93"/>
+      <c r="D39" s="93"/>
+      <c r="E39" s="93"/>
+      <c r="F39" s="93"/>
+      <c r="G39" s="93"/>
+      <c r="H39" s="87"/>
       <c r="I39" s="33"/>
-      <c r="J39" s="93"/>
-      <c r="K39" s="94"/>
-      <c r="L39" s="94"/>
-      <c r="M39" s="95"/>
+      <c r="J39" s="92"/>
+      <c r="K39" s="93"/>
+      <c r="L39" s="93"/>
+      <c r="M39" s="94"/>
     </row>
     <row r="40" spans="1:13" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="47"/>
-      <c r="B40" s="112"/>
-      <c r="C40" s="97"/>
-      <c r="D40" s="97"/>
-      <c r="E40" s="97"/>
-      <c r="F40" s="97"/>
-      <c r="G40" s="97"/>
-      <c r="H40" s="113"/>
+      <c r="B40" s="111"/>
+      <c r="C40" s="96"/>
+      <c r="D40" s="96"/>
+      <c r="E40" s="96"/>
+      <c r="F40" s="96"/>
+      <c r="G40" s="96"/>
+      <c r="H40" s="112"/>
       <c r="I40" s="34"/>
-      <c r="J40" s="96"/>
-      <c r="K40" s="97"/>
-      <c r="L40" s="97"/>
-      <c r="M40" s="98"/>
+      <c r="J40" s="95"/>
+      <c r="K40" s="96"/>
+      <c r="L40" s="96"/>
+      <c r="M40" s="97"/>
     </row>
   </sheetData>
   <protectedRanges>
-    <protectedRange sqref="I12 I11:J11 L11 A11:C11 K11:K12 D11:H13 G17:H17 J17 I13:M13 A30:M31 G15:J16 C13:C18 D14:J14 G21:H21 J21 G18:J20 A13:B27 C20:C22 G25:H25 J25 G22:J24 D15:F29 C24:C26 A28:C29 G29:H29 J29 G26:J28 K14:M29" name="Rango1"/>
-    <protectedRange sqref="I17 I21 I25 I29" name="Rango1_1"/>
+    <protectedRange sqref="I12 I11:J11 L11 A11:C11 K11:K12 D11:H13 I13:M13 A30:M31 C13:C18 A13:B27 C20:C22 D15:F25 C24:C25 G28:H28 G29:M29 C26:F27 A28:F29 D14:J14 J17 K14:M28 J28 G15:J16 G17:H17 G18:J27" name="Rango1"/>
+    <protectedRange sqref="I17 I28" name="Rango1_1"/>
   </protectedRanges>
-  <mergeCells count="43">
+  <mergeCells count="39">
     <mergeCell ref="J35:M35"/>
     <mergeCell ref="J36:M36"/>
     <mergeCell ref="J37:M37"/>
@@ -2987,13 +2915,9 @@
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="D11:I11"/>
     <mergeCell ref="A11:A31"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="C26:C29"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:C10" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Presencial, virtual, bimodal, a distancia, dual"</formula1>
     </dataValidation>
@@ -3003,23 +2927,30 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="B34" r:id="rId1" display="https://sistemascomputacionales.readthedocs.io/es/v2022.20" xr:uid="{F483E0E0-E4A7-4C2F-860A-EBA3E7D139F7}"/>
-    <hyperlink ref="K13" r:id="rId2" xr:uid="{D6255421-56CE-4DA6-B03E-76DEDA9FDF65}"/>
-    <hyperlink ref="K14:K28" r:id="rId3" display="https://sistemasfisicosinteractivos2.readthedocs.io/" xr:uid="{DC8141A9-F42B-4F45-841A-4DDD3E73F648}"/>
-    <hyperlink ref="K18:K21" r:id="rId4" display="https://sistemasfisicosinteractivos2.readthedocs.io/" xr:uid="{1631B9DA-9C6C-4D3E-8FB2-9BA7C96CE669}"/>
-    <hyperlink ref="K22:K25" r:id="rId5" display="https://sistemasfisicosinteractivos2.readthedocs.io/" xr:uid="{0D2B7084-9977-4A1D-8D38-0131CC30CA2E}"/>
-    <hyperlink ref="K26:K29" r:id="rId6" display="https://sistemasfisicosinteractivos2.readthedocs.io/" xr:uid="{2CAF67A0-003F-4B25-B53D-0C7C45425727}"/>
+    <hyperlink ref="K13" r:id="rId2" xr:uid="{A4C42719-E64A-4FB6-909A-49ECBF46C993}"/>
+    <hyperlink ref="K14:K28" r:id="rId3" display="https://sistemasfisicosinteractivos2.readthedocs.io/" xr:uid="{C864DA50-F16E-4BBA-A779-6C91E27911D8}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="1.2736614173228347" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="50" orientation="landscape" r:id="rId7"/>
+  <pageSetup paperSize="9" scale="50" orientation="landscape" r:id="rId4"/>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="13" max="53" man="1"/>
   </colBreaks>
-  <legacyDrawing r:id="rId8"/>
+  <legacyDrawing r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_activity xmlns="475903d6-5b88-4d7a-ba78-d123e191ef42" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010007385DC504DB614DA8F67D4315A28B14" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3ac3543c8bd13c0fc9dcbaaaa4f4e21f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="1be38a3c-13c4-46e0-8a29-91f320e906cc" xmlns:ns4="475903d6-5b88-4d7a-ba78-d123e191ef42" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="832580f857820fba5b25e66e4b08a8f5" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3277,7 +3208,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -3286,17 +3217,25 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_activity xmlns="475903d6-5b88-4d7a-ba78-d123e191ef42" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDE66BE-7C4D-4D57-9569-773F449FD84D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="1be38a3c-13c4-46e0-8a29-91f320e906cc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="475903d6-5b88-4d7a-ba78-d123e191ef42"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C325370-FB0B-42DC-B685-563E2C80434A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3316,28 +3255,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{635976DF-2941-4508-B3B6-F1CF25643BD3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDE66BE-7C4D-4D57-9569-773F449FD84D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="1be38a3c-13c4-46e0-8a29-91f320e906cc"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="475903d6-5b88-4d7a-ba78-d123e191ef42"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>